<commit_message>
Patched initialization of IEEEG1
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_ieeeg1.xlsx
+++ b/andes/cases/kundur/kundur_ieeeg1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAFC54D-E513-EA42-97E2-57FA752F768E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857CF7FD-4437-5949-8729-16F0DD69C8E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36740" yWindow="8540" windowWidth="24100" windowHeight="12100" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -3399,7 +3399,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3537,7 +3537,7 @@
         <v>0.4</v>
       </c>
       <c r="R2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -3546,7 +3546,7 @@
         <v>10</v>
       </c>
       <c r="U2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -3617,7 +3617,7 @@
         <v>0.4</v>
       </c>
       <c r="R3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -3626,7 +3626,7 @@
         <v>10</v>
       </c>
       <c r="U3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -3700,7 +3700,7 @@
         <v>0.4</v>
       </c>
       <c r="R4">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -3709,7 +3709,7 @@
         <v>10</v>
       </c>
       <c r="U4">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -3721,7 +3721,7 @@
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="Z4">
         <v>0.1</v>
@@ -3730,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>